<commit_message>
Fix HTTPRequest activity without asset
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\GetJiraSlaReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFD21C5-9E05-4D7C-AA2B-5F36A806C0BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0B8861-EEE2-4D3C-AE2D-7CDF5B65C844}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36360" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -149,9 +149,6 @@
     <t>OulookAccountRobot</t>
   </si>
   <si>
-    <t>n.but@qiwi.com</t>
-  </si>
-  <si>
     <t>AssetName</t>
   </si>
   <si>
@@ -288,9 +285,6 @@
   </si>
   <si>
     <t>Data\Input\</t>
-  </si>
-  <si>
-    <t>Data\Output\</t>
   </si>
   <si>
     <t>qiwi.com</t>
@@ -365,9 +359,6 @@
   </si>
   <si>
     <t>Fill this field if not using orchestrator asset</t>
-  </si>
-  <si>
-    <t>smtp1.osmp.ru</t>
   </si>
   <si>
     <t>OulookSMTPPort</t>
@@ -398,9 +389,6 @@
 {3} - list of employees for filtering tickets</t>
   </si>
   <si>
-    <t>1cuipath_bot</t>
-  </si>
-  <si>
     <t>project = {0} AND updated &gt;= {1} AND updated &lt;= {2} AND assignee in ({3}) ORDER BY created ASC</t>
   </si>
   <si>
@@ -427,9 +415,6 @@
   </si>
   <si>
     <t>This folder was separated from robot folder because client should update employees list and schedule. So give this file to client and change this path to client's folder</t>
-  </si>
-  <si>
-    <t>rbt-88</t>
   </si>
   <si>
     <t>Orchestrator queue name. Leave empty if prefer use local without Orchestrator Queue</t>
@@ -465,14 +450,29 @@
     </r>
   </si>
   <si>
-    <t>testaccountrandomcompany@testmailrandomcompany.com</t>
+    <t>JiraCredAsset</t>
+  </si>
+  <si>
+    <t>QueueName</t>
+  </si>
+  <si>
+    <t>support@mail.com</t>
+  </si>
+  <si>
+    <t>robot@mail.com</t>
+  </si>
+  <si>
+    <t>manager@mail.com</t>
+  </si>
+  <si>
+    <t>Data\Output\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -522,11 +522,6 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -586,7 +581,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -603,7 +598,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -631,7 +625,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -951,7 +945,7 @@
   <dimension ref="A1:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,420 +992,418 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>133</v>
+      <c r="B3" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>123</v>
+      <c r="A4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>113</v>
+      <c r="A6" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>118</v>
+      <c r="A8" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="3" t="s">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>75</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="B36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="C38" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="3" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>54</v>
+      <c r="A43" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="B43" s="1">
         <v>180</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>55</v>
+      <c r="A47" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="B47" s="1">
         <v>5400</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1430,221 +1422,221 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" style="8" customWidth="1"/>
-    <col min="27" max="16384" width="14.42578125" style="8"/>
+    <col min="1" max="1" width="35.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" style="7" customWidth="1"/>
+    <col min="27" max="16384" width="14.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>108</v>
+      <c r="C3" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="10"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>3000</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>15000</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>30000</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>0.6</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>0.8</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>0.9</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="10"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>